<commit_message>
feat: Update Ajay.xslx Initialize atoms assignment - Update Ajay.xlsx
</commit_message>
<xml_diff>
--- a/atoms_assignment/Ajay.xlsx
+++ b/atoms_assignment/Ajay.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Atoms</t>
   </si>
@@ -29,7 +29,7 @@
   </si>
   <si>
     <t>text input field
-button 
+button (login)
 icon
 text element</t>
   </si>
@@ -55,16 +55,18 @@
     <t>google login dialog box</t>
   </si>
   <si>
-    <t>login page(google)</t>
-  </si>
-  <si>
-    <t>image/avatar</t>
+    <t>login page(google)/sign up page</t>
+  </si>
+  <si>
+    <t>image/profile avatar
+cashkick buttons and learn more</t>
   </si>
   <si>
     <t>slidebar navigation , notification card , action card and payment summary</t>
   </si>
   <si>
-    <t>header , main , content area , sidebar</t>
+    <t>header , main , content area , sidebar
+side navigation bar , alerts(cashkick)</t>
   </si>
   <si>
     <t>home page layout</t>
@@ -77,10 +79,17 @@
 cards : term cap , available credit , max interest rate </t>
   </si>
   <si>
+    <t>acceleration table</t>
+  </si>
+  <si>
     <t>cash acceleration page layout</t>
   </si>
   <si>
     <t>cash accelaration page</t>
+  </si>
+  <si>
+    <t>buttons for reset , back navigation 
+and credit review</t>
   </si>
   <si>
     <t>slider for auto-selection and financial details
@@ -96,6 +105,9 @@
     <t>cask kick page (new)</t>
   </si>
   <si>
+    <t>button (cancel)</t>
+  </si>
+  <si>
     <t>cash kick form</t>
   </si>
   <si>
@@ -108,6 +120,21 @@
     <t>cask kick page (name)</t>
   </si>
   <si>
+    <t>logout , settings ,payments</t>
+  </si>
+  <si>
+    <t>popup(avatar)</t>
+  </si>
+  <si>
+    <t>dashboard layout</t>
+  </si>
+  <si>
+    <t>dashboard page</t>
+  </si>
+  <si>
+    <t>review element</t>
+  </si>
+  <si>
     <t>success dialog</t>
   </si>
   <si>
@@ -115,6 +142,48 @@
   </si>
   <si>
     <t>success dialog page</t>
+  </si>
+  <si>
+    <t>reset button</t>
+  </si>
+  <si>
+    <t>form for forgot password</t>
+  </si>
+  <si>
+    <t>reset password</t>
+  </si>
+  <si>
+    <t>forgot password layout</t>
+  </si>
+  <si>
+    <t>login page(password forgot)</t>
+  </si>
+  <si>
+    <t>continue button</t>
+  </si>
+  <si>
+    <t>reset email item</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>change password form</t>
+  </si>
+  <si>
+    <t>change password</t>
+  </si>
+  <si>
+    <t>change password layout</t>
+  </si>
+  <si>
+    <t>login button</t>
+  </si>
+  <si>
+    <t>password reset item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login </t>
   </si>
 </sst>
 </file>
@@ -396,11 +465,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.63"/>
+    <col customWidth="1" min="1" max="1" width="25.5"/>
     <col customWidth="1" min="2" max="2" width="57.13"/>
     <col customWidth="1" min="3" max="3" width="33.13"/>
     <col customWidth="1" min="4" max="4" width="22.25"/>
-    <col customWidth="1" min="5" max="5" width="22.88"/>
+    <col customWidth="1" min="5" max="5" width="25.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -472,50 +541,138 @@
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>